<commit_message>
Seperated Requests into A and B. Everything should be OK there
</commit_message>
<xml_diff>
--- a/Files/50000-51000/50282/A50282_RequestList.xlsx
+++ b/Files/50000-51000/50282/A50282_RequestList.xlsx
@@ -25,7 +25,7 @@
     <t>ОФИС гр. РУСЕ и ОФИС гр. СОФИЯ</t>
   </si>
   <si>
-    <t>ЗАЯВКА № A50282 / Дата 28.06.2016</t>
+    <t>ЗАЯВКА № A50282 / Дата 03.07.2016</t>
   </si>
   <si>
     <t>7.1 МИКРОБИОЛОГИЧНО ИЗПИТВАНЕ</t>
@@ -82,7 +82,7 @@
     <t>БДС EN ISO 4833-1:2013</t>
   </si>
   <si>
-    <t>Срок за изпитване: 4 дни</t>
+    <t>Срок за изпитване: 7 дни</t>
   </si>
   <si>
     <t>Приел пробата......</t>

</xml_diff>